<commit_message>
Data updated 13/4 12:00
</commit_message>
<xml_diff>
--- a/data/muestras.xlsx
+++ b/data/muestras.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eloy\Desktop\COVID 19\Dashboard\dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0456829E-678C-4014-A28E-88D1CABB6929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDE6DEE-1FCE-49E4-9F67-24704817DD6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$136</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="12">
   <si>
     <t>NEG-COVID-19</t>
   </si>
@@ -461,13 +472,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B128" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F136" sqref="F136"/>
+      <selection pane="bottomRight" activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1296,7 +1307,7 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1411,7 +1422,7 @@
         <v>8</v>
       </c>
       <c r="D41">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1687,7 +1698,7 @@
         <v>5</v>
       </c>
       <c r="D53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1756,7 +1767,7 @@
         <v>8</v>
       </c>
       <c r="D56">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1871,7 +1882,7 @@
         <v>8</v>
       </c>
       <c r="D61">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -1894,7 +1905,7 @@
         <v>4</v>
       </c>
       <c r="D62">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -2009,7 +2020,7 @@
         <v>4</v>
       </c>
       <c r="D67">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -2124,7 +2135,7 @@
         <v>4</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -2216,7 +2227,7 @@
         <v>8</v>
       </c>
       <c r="D76">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -2248,7 +2259,7 @@
         <v>0</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2262,7 +2273,7 @@
         <v>5</v>
       </c>
       <c r="D78">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -2331,7 +2342,7 @@
         <v>8</v>
       </c>
       <c r="D81">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2446,7 +2457,7 @@
         <v>8</v>
       </c>
       <c r="D86">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -2469,7 +2480,7 @@
         <v>4</v>
       </c>
       <c r="D87">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -2561,7 +2572,7 @@
         <v>8</v>
       </c>
       <c r="D91">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -2584,7 +2595,7 @@
         <v>4</v>
       </c>
       <c r="D92">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -2593,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2676,7 +2687,7 @@
         <v>8</v>
       </c>
       <c r="D96">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -2685,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3608,7 +3619,124 @@
         <v>0</v>
       </c>
     </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C137" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137">
+        <v>66</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C138" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138">
+        <v>22</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C139" t="s">
+        <v>4</v>
+      </c>
+      <c r="D139">
+        <v>17</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C140" t="s">
+        <v>8</v>
+      </c>
+      <c r="D140">
+        <v>39</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C141" t="s">
+        <v>5</v>
+      </c>
+      <c r="D141">
+        <v>40</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>2</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:G136" xr:uid="{52B0F4C3-943B-4C06-8F28-ED7C0550389F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anotaciones en algunas graficas, actualizacion de los datos del dia 21
</commit_message>
<xml_diff>
--- a/data/muestras.xlsx
+++ b/data/muestras.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eloy\Desktop\COVID 19\Dashboard\dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED64306-5796-4725-B80C-891F205423ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6103AB-E531-456C-9A4A-0CA6F6526994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="12">
   <si>
     <t>NEG-COVID-19</t>
   </si>
@@ -486,13 +486,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B156" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B165" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D167" sqref="D167:G171"/>
+      <selection pane="bottomRight" activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4438,6 +4438,221 @@
         <v>0</v>
       </c>
     </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="3">
+        <v>170</v>
+      </c>
+      <c r="B172" s="2">
+        <v>43941</v>
+      </c>
+      <c r="C172" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172">
+        <v>31</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="3">
+        <v>171</v>
+      </c>
+      <c r="B173" s="2">
+        <v>43941</v>
+      </c>
+      <c r="C173" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="3">
+        <v>172</v>
+      </c>
+      <c r="B174" s="2">
+        <v>43941</v>
+      </c>
+      <c r="C174" t="s">
+        <v>4</v>
+      </c>
+      <c r="D174">
+        <v>13</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+      <c r="G174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="3">
+        <v>173</v>
+      </c>
+      <c r="B175" s="2">
+        <v>43941</v>
+      </c>
+      <c r="C175" t="s">
+        <v>8</v>
+      </c>
+      <c r="D175">
+        <v>119</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="G175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="3">
+        <v>174</v>
+      </c>
+      <c r="B176" s="2">
+        <v>43941</v>
+      </c>
+      <c r="C176" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176">
+        <v>22</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="G176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="3">
+        <v>175</v>
+      </c>
+      <c r="B177" s="2">
+        <v>43942</v>
+      </c>
+      <c r="C177" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177">
+        <v>25</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="3">
+        <v>176</v>
+      </c>
+      <c r="B178" s="2">
+        <v>43942</v>
+      </c>
+      <c r="C178" t="s">
+        <v>6</v>
+      </c>
+      <c r="D178">
+        <v>131</v>
+      </c>
+      <c r="F178">
+        <v>1</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="3">
+        <v>177</v>
+      </c>
+      <c r="B179" s="2">
+        <v>43942</v>
+      </c>
+      <c r="C179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D179">
+        <v>5</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="3">
+        <v>178</v>
+      </c>
+      <c r="B180" s="2">
+        <v>43942</v>
+      </c>
+      <c r="C180" t="s">
+        <v>8</v>
+      </c>
+      <c r="D180">
+        <v>89</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="3">
+        <v>179</v>
+      </c>
+      <c r="B181" s="2">
+        <v>43942</v>
+      </c>
+      <c r="C181" t="s">
+        <v>5</v>
+      </c>
+      <c r="D181">
+        <v>30</v>
+      </c>
+      <c r="F181">
+        <v>1</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G136" xr:uid="{52B0F4C3-943B-4C06-8F28-ED7C0550389F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>